<commit_message>
update word count function
</commit_message>
<xml_diff>
--- a/materials/workshop/excel-examples.xlsx
+++ b/materials/workshop/excel-examples.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Documents/GitHub/apra-intro-to-text-mining/materials/workshop/02-excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Documents/GitHub/text-mining-workshop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA06E98-A4FB-944A-9431-F0093B5B3424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70876973-0908-AF4C-8B5B-0C7B40F876CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="28360" windowHeight="18380" xr2:uid="{B1724EF6-6E2D-43A9-93AA-4F3B51A5441F}"/>
   </bookViews>
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D993A40E-E1B7-3B49-87F3-8B406BFE1920}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -683,8 +683,8 @@
         <v>40</v>
       </c>
       <c r="C2" s="9">
-        <f>LEN(A2)-LEN(SUBSTITUTE(A2," ",""))+1</f>
-        <v>8</v>
+        <f>LEN(TRIM(A2))-LEN(SUBSTITUTE(A2," ",""))+1</f>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="64" x14ac:dyDescent="0.2">

</xml_diff>